<commit_message>
is it over? yes almost
</commit_message>
<xml_diff>
--- a/symbols and abbrevs.xlsx
+++ b/symbols and abbrevs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arjan\Desktop\thesis\thesis-report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87FA8049-8152-4172-9205-A12FEC9F7982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F605F7-6284-432E-9F9C-6070A6AD4BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2250" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8527BC41-47B2-466B-992D-80F7F8310EED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{8527BC41-47B2-466B-992D-80F7F8310EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="182">
   <si>
     <t>Unit</t>
   </si>
@@ -58,9 +59,6 @@
     <t>pv</t>
   </si>
   <si>
-    <t>albedo</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -82,18 +80,9 @@
     <t>Signal-to-noise ratio</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
     <t>b</t>
   </si>
   <si>
-    <t>latitude</t>
-  </si>
-  <si>
     <t>deg</t>
   </si>
   <si>
@@ -127,9 +116,6 @@
     <t>flux</t>
   </si>
   <si>
-    <t>Wm-2</t>
-  </si>
-  <si>
     <t>NEATM</t>
   </si>
   <si>
@@ -145,15 +131,6 @@
     <t>alpha</t>
   </si>
   <si>
-    <t>phase angle</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>signal</t>
-  </si>
-  <si>
     <t>e-</t>
   </si>
   <si>
@@ -169,9 +146,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>number</t>
-  </si>
-  <si>
     <t>S/C</t>
   </si>
   <si>
@@ -211,22 +185,403 @@
     <t>theta</t>
   </si>
   <si>
-    <t>true anomaly</t>
-  </si>
-  <si>
     <t>Omega</t>
   </si>
   <si>
     <t>omega</t>
   </si>
   <si>
-    <t>Right ascenscion of the ascending node</t>
-  </si>
-  <si>
-    <t>Argument of periapsis</t>
-  </si>
-  <si>
     <t>Abbrevations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number </t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Palomar-Leiden exponent</t>
+  </si>
+  <si>
+    <t>assumed albedo</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Catalina Sky Survey</t>
+  </si>
+  <si>
+    <t>LSST</t>
+  </si>
+  <si>
+    <t>Large Synoptic Survey Telescope</t>
+  </si>
+  <si>
+    <t>ATLAS</t>
+  </si>
+  <si>
+    <t>Asteroid Terrestrial-Impact Last Alert System</t>
+  </si>
+  <si>
+    <t>WISE</t>
+  </si>
+  <si>
+    <t>Widefield Infrared Survey Explorer</t>
+  </si>
+  <si>
+    <t>NEOWISE</t>
+  </si>
+  <si>
+    <t>Near-Earth Object WISE</t>
+  </si>
+  <si>
+    <t>NEOCam</t>
+  </si>
+  <si>
+    <t>Near-Earth Object Camera</t>
+  </si>
+  <si>
+    <t>NASA</t>
+  </si>
+  <si>
+    <t>National Aeronautics and Space Administration</t>
+  </si>
+  <si>
+    <t>JPL</t>
+  </si>
+  <si>
+    <t>Jet Propulsion Laboratory</t>
+  </si>
+  <si>
+    <t>L1, L2, L3</t>
+  </si>
+  <si>
+    <t>Lagrange Points</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>heliocentric ecliptic longitude</t>
+  </si>
+  <si>
+    <t>heliocentric ecliptic latitude</t>
+  </si>
+  <si>
+    <t>lg</t>
+  </si>
+  <si>
+    <t>bg</t>
+  </si>
+  <si>
+    <t>galactic longitude</t>
+  </si>
+  <si>
+    <t>galactic latitude</t>
+  </si>
+  <si>
+    <t>bNGP</t>
+  </si>
+  <si>
+    <t>laittude of the North Galactic Pole</t>
+  </si>
+  <si>
+    <t>lNGP</t>
+  </si>
+  <si>
+    <t>ascending node of the Milky Way</t>
+  </si>
+  <si>
+    <t>lGC</t>
+  </si>
+  <si>
+    <t>longitude of the Galactic Core</t>
+  </si>
+  <si>
+    <t>heliocentric, ecliptic reference frame</t>
+  </si>
+  <si>
+    <t>body-centered, ecliptic reference frame</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>body-centered, ecliptic reference frame oriented w.r.t. the Sun</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>galactic reference frame</t>
+  </si>
+  <si>
+    <t>odot</t>
+  </si>
+  <si>
+    <t>the Sun</t>
+  </si>
+  <si>
+    <t>oplus</t>
+  </si>
+  <si>
+    <t>the Earth</t>
+  </si>
+  <si>
+    <t>n_c</t>
+  </si>
+  <si>
+    <t>density of component c</t>
+  </si>
+  <si>
+    <t>particles/AU</t>
+  </si>
+  <si>
+    <t>Ec</t>
+  </si>
+  <si>
+    <t>emissivity of component c</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>W/m2</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>COBE</t>
+  </si>
+  <si>
+    <t>Cosmic Background Explorer</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>angular distance from the subsolar point</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>bond albedo</t>
+  </si>
+  <si>
+    <t>F odot</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>Stefan-Boltzmann constant</t>
+  </si>
+  <si>
+    <t>Wm-2K-4</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>beaming parameter</t>
+  </si>
+  <si>
+    <t>solar phase angle</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>heliocentric distance of target</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>distance from target to observer</t>
+  </si>
+  <si>
+    <t>CCD</t>
+  </si>
+  <si>
+    <t>Charge-coupled device</t>
+  </si>
+  <si>
+    <t>St</t>
+  </si>
+  <si>
+    <t>target signal</t>
+  </si>
+  <si>
+    <t>Sb</t>
+  </si>
+  <si>
+    <t>Background signal</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>tau</t>
+  </si>
+  <si>
+    <t>integration time</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>kf</t>
+  </si>
+  <si>
+    <t>straddle factor</t>
+  </si>
+  <si>
+    <t>Qe</t>
+  </si>
+  <si>
+    <t>quantum efficiency</t>
+  </si>
+  <si>
+    <t>planck constant</t>
+  </si>
+  <si>
+    <t>JHz-1</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>speed of light</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>meaning</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>dark current</t>
+  </si>
+  <si>
+    <t>readout noise</t>
+  </si>
+  <si>
+    <t>e-/s</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>field of view</t>
+  </si>
+  <si>
+    <t>deg2</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>s-1</t>
+  </si>
+  <si>
+    <t>angular size</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>ANN</t>
+  </si>
+  <si>
+    <t>Artificial Neural Network</t>
+  </si>
+  <si>
+    <t>mean anomaly at epoch</t>
+  </si>
+  <si>
+    <t>inter-spacecraft spread</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>AU2</t>
+  </si>
+  <si>
+    <t>Atotal</t>
+  </si>
+  <si>
+    <t>total area</t>
+  </si>
+  <si>
+    <t>CURR</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>PROJ</t>
+  </si>
+  <si>
+    <t>projection</t>
+  </si>
+  <si>
+    <t>argument of periapsis</t>
+  </si>
+  <si>
+    <t>phi max</t>
+  </si>
+  <si>
+    <t>Delta theta</t>
+  </si>
+  <si>
+    <t>Solar flux at 1 AU</t>
+  </si>
+  <si>
+    <t>aperture</t>
+  </si>
+  <si>
+    <t>area covered at magnitude H</t>
+  </si>
+  <si>
+    <t>reference temperature</t>
+  </si>
+  <si>
+    <t>zodiacal flux</t>
+  </si>
+  <si>
+    <t>maximum solar elongation</t>
+  </si>
+  <si>
+    <t>right ascension of the ascending node</t>
+  </si>
+  <si>
+    <t>2.95 to 3.5</t>
   </si>
 </sst>
 </file>
@@ -262,8 +617,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6DAE93-80D7-44AD-B6DF-F139A2A92272}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C21"/>
+      <selection sqref="A1:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,238 +961,680 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
         <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
         <v>19</v>
       </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>177</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>178</v>
+      </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>172</v>
+      </c>
+      <c r="B40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C22">
-    <sortCondition ref="A1:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C49">
+    <sortCondition ref="A1:A49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F913808D-FDF8-4328-998F-9EA976B487BE}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3EF4DB-5D3C-4F55-86C2-05786D52E0CD}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection sqref="A1:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2">
+        <v>6.6260701500000003</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3">
+        <v>299792458</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.6699999999999998E-8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>29.81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7">
+        <v>270.02</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8">
+        <v>6.38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9">
+        <v>1351</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F913808D-FDF8-4328-998F-9EA976B487BE}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,7 +1645,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -854,55 +1653,215 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B9">
-    <sortCondition ref="A1:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B25">
+    <sortCondition ref="A1:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>